<commit_message>
Added rudimentary industry STEEL and OTHER functionality
* industry gridConnection types STEEL and OTHER toegevoegd voor GCIndustry in backBoneConfig300 excel. Deze worden ook aangemaakt bij model configuration.
* profielen voor elektriciteits- en warmtevraag updaten elk uur voor industry STEEL en OTHER.
* bijbehorende defaultEnergyAssets toegevoegd voor electriciteitsvraag en warmtevraag.
* defaultEnergyAssets methane_furnace en hydrogen_furnace voor de industry toegevoegd.
* J_EAConversionHydrogenBurner toegevoegd, analoog aan GasBurner.
* GCIndustry agent: simpele energyAsset aansturing toegevoegd voor consumption assets en conversion assets.
BUG: dubbeltelling flows in GCIndustry als warmtevraag wordt bepaald en vervolgens ingevuld met conversionasset!
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig_300.xlsx
+++ b/Base/db_backboneConfig_300.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BCCAEC-A20F-4DA2-A24B-08F1F58CD8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7024EF-51E9-42DB-B525-5A18C406606E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3788" uniqueCount="671">
   <si>
     <t>id</t>
   </si>
@@ -2028,6 +2028,30 @@
   </si>
   <si>
     <t>isolation_label</t>
+  </si>
+  <si>
+    <t>b301</t>
+  </si>
+  <si>
+    <t>b302</t>
+  </si>
+  <si>
+    <t>INDUSTRY</t>
+  </si>
+  <si>
+    <t>STEEL</t>
+  </si>
+  <si>
+    <t>com9</t>
+  </si>
+  <si>
+    <t>com10</t>
+  </si>
+  <si>
+    <t>INDUSTRY_OTHER</t>
+  </si>
+  <si>
+    <t>HYDROGENFIRED</t>
   </si>
 </sst>
 </file>
@@ -2625,10 +2649,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F79AE7D-6C5C-4EEF-8F2D-727C87414EF2}">
-  <dimension ref="A1:K301"/>
+  <dimension ref="A1:K303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="H306" sqref="H306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2638,6 +2662,7 @@
     <col min="5" max="5" width="23.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -12474,6 +12499,70 @@
       </c>
       <c r="K301" t="s">
         <v>641</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>300</v>
+      </c>
+      <c r="B302" t="s">
+        <v>650</v>
+      </c>
+      <c r="C302" t="s">
+        <v>663</v>
+      </c>
+      <c r="D302" t="s">
+        <v>665</v>
+      </c>
+      <c r="E302" t="s">
+        <v>666</v>
+      </c>
+      <c r="F302" t="s">
+        <v>103</v>
+      </c>
+      <c r="G302" t="s">
+        <v>647</v>
+      </c>
+      <c r="H302" t="s">
+        <v>1</v>
+      </c>
+      <c r="J302">
+        <v>1000</v>
+      </c>
+      <c r="K302" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>301</v>
+      </c>
+      <c r="B303" t="s">
+        <v>650</v>
+      </c>
+      <c r="C303" t="s">
+        <v>664</v>
+      </c>
+      <c r="D303" t="s">
+        <v>665</v>
+      </c>
+      <c r="E303" t="s">
+        <v>669</v>
+      </c>
+      <c r="F303" t="s">
+        <v>103</v>
+      </c>
+      <c r="G303" t="s">
+        <v>670</v>
+      </c>
+      <c r="H303" t="s">
+        <v>2</v>
+      </c>
+      <c r="J303">
+        <v>1000</v>
+      </c>
+      <c r="K303" t="s">
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -12484,10 +12573,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F595F011-BCBA-42A0-B2C1-EC2B9C01AA0D}">
-  <dimension ref="A1:E293"/>
+  <dimension ref="A1:E295"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="C302" sqref="C302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -17475,6 +17564,40 @@
         <v>91</v>
       </c>
     </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>292</v>
+      </c>
+      <c r="B294" t="s">
+        <v>93</v>
+      </c>
+      <c r="C294" t="s">
+        <v>101</v>
+      </c>
+      <c r="D294" t="s">
+        <v>667</v>
+      </c>
+      <c r="E294" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>293</v>
+      </c>
+      <c r="B295" t="s">
+        <v>93</v>
+      </c>
+      <c r="C295" t="s">
+        <v>101</v>
+      </c>
+      <c r="D295" t="s">
+        <v>668</v>
+      </c>
+      <c r="E295" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17486,7 +17609,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Data agnostic policy configuration
*Policies niet meer hardcoden maar extern configureren, in een nieuwe tab in de backBoneConfig excel!
*Python-scripts aangepast: experimenten bevatten nu ook policy-configs, worden ook omgezet in JSON-string.
*Policy values worden uit JSON-string ingelezen on model startup en waarden worden centraal geset in de betreffende agents.
*Nu geïmplementeerd: default charging behavior voor EVs (CHEAP), gridOperator congestion policy values (o.a. congestion thresholds en tarieven, boolean wel of niet congestionpricing toepassen voor consumption en production)
*Nieuwe policy-waarden kunnen zo eenvoudig en generiek data-agnost toegevoegd worden aan het model
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig_300.xlsx
+++ b/Base/db_backboneConfig_300.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7024EF-51E9-42DB-B525-5A18C406606E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61FB24C-485F-4E94-AE3F-1CB367F201E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="config_gridConnections" sheetId="7" r:id="rId3"/>
     <sheet name="config_actors" sheetId="5" r:id="rId4"/>
     <sheet name="config_energyAssets" sheetId="4" r:id="rId5"/>
+    <sheet name="config_policies" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3788" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3809" uniqueCount="687">
   <si>
     <t>id</t>
   </si>
@@ -2052,6 +2053,54 @@
   </si>
   <si>
     <t>HYDROGENFIRED</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>EV_charging_attitude_standard</t>
+  </si>
+  <si>
+    <t>CHEAP</t>
+  </si>
+  <si>
+    <t>charging behaviour not contingent on holon</t>
+  </si>
+  <si>
+    <t>Grid_MS_congestion_allowance_level_kW</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>gridOperator policy variable</t>
+  </si>
+  <si>
+    <t>Grid_MS_congestion_price</t>
+  </si>
+  <si>
+    <t>gridOperator policy value</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>Grid_MS_congestion_threshold</t>
+  </si>
+  <si>
+    <t>Grid_MS_congestion_pricing_consumption</t>
+  </si>
+  <si>
+    <t>Grid_MS_congestion_pricing_production</t>
   </si>
 </sst>
 </file>
@@ -2651,7 +2700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F79AE7D-6C5C-4EEF-8F2D-727C87414EF2}">
   <dimension ref="A1:K303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
+    <sheetView topLeftCell="A271" workbookViewId="0">
       <selection activeCell="H306" sqref="H306"/>
     </sheetView>
   </sheetViews>
@@ -17961,4 +18010,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F811909-04C9-49BC-AE7A-FC0724E3AC0A}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>671</v>
+      </c>
+      <c r="C1" t="s">
+        <v>672</v>
+      </c>
+      <c r="D1" t="s">
+        <v>673</v>
+      </c>
+      <c r="E1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>675</v>
+      </c>
+      <c r="C2" t="s">
+        <v>676</v>
+      </c>
+      <c r="E2" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>678</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>679</v>
+      </c>
+      <c r="E3" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>681</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>679</v>
+      </c>
+      <c r="E4" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>684</v>
+      </c>
+      <c r="C5">
+        <v>0.7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>683</v>
+      </c>
+      <c r="E5" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>685</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>686</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>682</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DH with heatpump and boiler functional
Some changes to the J_EAConversionHeatPump class to have correct results from getHeatCapacity_kW() method

Parameters not yet tuned, at the moment boiler is not being used yet. Also, no 'opportunity heating' active as there is not yet any energySurpluss variable that can be used for that.
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig_300.xlsx
+++ b/Base/db_backboneConfig_300.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61FB24C-485F-4E94-AE3F-1CB367F201E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C6EF90-213E-4CC7-9E6A-EE32F1124B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="28470" windowHeight="16920" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3809" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3809" uniqueCount="688">
   <si>
     <t>id</t>
   </si>
@@ -2101,6 +2101,9 @@
   </si>
   <si>
     <t>Grid_MS_congestion_pricing_production</t>
+  </si>
+  <si>
+    <t>HEATPUMP_BOILERPEAK</t>
   </si>
 </sst>
 </file>
@@ -2700,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F79AE7D-6C5C-4EEF-8F2D-727C87414EF2}">
   <dimension ref="A1:K303"/>
   <sheetViews>
-    <sheetView topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="H306" sqref="H306"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3648,7 +3651,7 @@
         <v>103</v>
       </c>
       <c r="G29" t="s">
-        <v>647</v>
+        <v>687</v>
       </c>
       <c r="H29" t="s">
         <v>2</v>
@@ -18016,7 +18019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F811909-04C9-49BC-AE7A-FC0724E3AC0A}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
District Heating system H1 applies opportunity heating based on electricity surpluss of energy Holon 1
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig_300.xlsx
+++ b/Base/db_backboneConfig_300.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C6EF90-213E-4CC7-9E6A-EE32F1124B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405E2B53-BC96-4889-B05C-C7996D739D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="28470" windowHeight="16920" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="18375" yWindow="3720" windowWidth="28470" windowHeight="16920" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3809" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3810" uniqueCount="688">
   <si>
     <t>id</t>
   </si>
@@ -2150,11 +2150,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2703,8 +2704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F79AE7D-6C5C-4EEF-8F2D-727C87414EF2}">
   <dimension ref="A1:K303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2714,6 +2715,7 @@
     <col min="5" max="5" width="23.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3663,7 +3665,7 @@
         <v>400000</v>
       </c>
       <c r="K29" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -12627,8 +12629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F595F011-BCBA-42A0-B2C1-EC2B9C01AA0D}">
   <dimension ref="A1:E295"/>
   <sheetViews>
-    <sheetView topLeftCell="A266" workbookViewId="0">
-      <selection activeCell="C302" sqref="C302"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -12651,7 +12653,7 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>87</v>
       </c>
     </row>
@@ -12668,7 +12670,7 @@
       <c r="D2" t="s">
         <v>69</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12685,7 +12687,7 @@
       <c r="D3" t="s">
         <v>70</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12702,7 +12704,7 @@
       <c r="D4" t="s">
         <v>71</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12719,7 +12721,7 @@
       <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12736,7 +12738,7 @@
       <c r="D6" t="s">
         <v>73</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12753,7 +12755,7 @@
       <c r="D7" t="s">
         <v>74</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12770,7 +12772,7 @@
       <c r="D8" t="s">
         <v>75</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12787,7 +12789,7 @@
       <c r="D9" t="s">
         <v>76</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12804,7 +12806,7 @@
       <c r="D10" t="s">
         <v>77</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12821,7 +12823,7 @@
       <c r="D11" t="s">
         <v>78</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12838,7 +12840,7 @@
       <c r="D12" t="s">
         <v>79</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12855,7 +12857,7 @@
       <c r="D13" t="s">
         <v>80</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12872,7 +12874,7 @@
       <c r="D14" t="s">
         <v>81</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12889,7 +12891,7 @@
       <c r="D15" t="s">
         <v>82</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12906,7 +12908,7 @@
       <c r="D16" t="s">
         <v>83</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12923,7 +12925,7 @@
       <c r="D17" t="s">
         <v>84</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12940,7 +12942,7 @@
       <c r="D18" t="s">
         <v>85</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12957,7 +12959,7 @@
       <c r="D19" t="s">
         <v>86</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12974,7 +12976,7 @@
       <c r="D20" t="s">
         <v>89</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>96</v>
       </c>
     </row>
@@ -12991,7 +12993,7 @@
       <c r="D21" t="s">
         <v>90</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13008,7 +13010,7 @@
       <c r="D22" t="s">
         <v>91</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="4" t="s">
         <v>97</v>
       </c>
     </row>
@@ -13025,7 +13027,7 @@
       <c r="D23" t="s">
         <v>92</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="4" t="s">
         <v>97</v>
       </c>
     </row>
@@ -13042,7 +13044,7 @@
       <c r="D24" t="s">
         <v>96</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -13059,6 +13061,9 @@
       <c r="D25" t="s">
         <v>643</v>
       </c>
+      <c r="E25" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -13073,7 +13078,7 @@
       <c r="D26" t="s">
         <v>104</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13090,8 +13095,8 @@
       <c r="D27" t="s">
         <v>105</v>
       </c>
-      <c r="E27" t="s">
-        <v>91</v>
+      <c r="E27" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -13107,7 +13112,7 @@
       <c r="D28" t="s">
         <v>106</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13124,8 +13129,8 @@
       <c r="D29" t="s">
         <v>107</v>
       </c>
-      <c r="E29" t="s">
-        <v>96</v>
+      <c r="E29" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -13141,7 +13146,7 @@
       <c r="D30" t="s">
         <v>108</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13158,7 +13163,7 @@
       <c r="D31" t="s">
         <v>109</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13175,7 +13180,7 @@
       <c r="D32" t="s">
         <v>110</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13192,7 +13197,7 @@
       <c r="D33" t="s">
         <v>111</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13209,8 +13214,8 @@
       <c r="D34" t="s">
         <v>112</v>
       </c>
-      <c r="E34" t="s">
-        <v>91</v>
+      <c r="E34" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -13226,8 +13231,8 @@
       <c r="D35" t="s">
         <v>113</v>
       </c>
-      <c r="E35" t="s">
-        <v>91</v>
+      <c r="E35" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -13243,8 +13248,8 @@
       <c r="D36" t="s">
         <v>114</v>
       </c>
-      <c r="E36" t="s">
-        <v>91</v>
+      <c r="E36" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -13260,7 +13265,7 @@
       <c r="D37" t="s">
         <v>115</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13277,7 +13282,7 @@
       <c r="D38" t="s">
         <v>116</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13294,7 +13299,7 @@
       <c r="D39" t="s">
         <v>117</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13311,7 +13316,7 @@
       <c r="D40" t="s">
         <v>118</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13328,7 +13333,7 @@
       <c r="D41" t="s">
         <v>119</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13345,7 +13350,7 @@
       <c r="D42" t="s">
         <v>120</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13362,7 +13367,7 @@
       <c r="D43" t="s">
         <v>121</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13379,7 +13384,7 @@
       <c r="D44" t="s">
         <v>122</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13396,8 +13401,8 @@
       <c r="D45" t="s">
         <v>123</v>
       </c>
-      <c r="E45" t="s">
-        <v>91</v>
+      <c r="E45" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -13413,7 +13418,7 @@
       <c r="D46" t="s">
         <v>124</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13430,7 +13435,7 @@
       <c r="D47" t="s">
         <v>125</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13447,7 +13452,7 @@
       <c r="D48" t="s">
         <v>126</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13464,7 +13469,7 @@
       <c r="D49" t="s">
         <v>127</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13481,7 +13486,7 @@
       <c r="D50" t="s">
         <v>128</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13498,7 +13503,7 @@
       <c r="D51" t="s">
         <v>129</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13515,8 +13520,8 @@
       <c r="D52" t="s">
         <v>130</v>
       </c>
-      <c r="E52" t="s">
-        <v>91</v>
+      <c r="E52" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -13532,8 +13537,8 @@
       <c r="D53" t="s">
         <v>131</v>
       </c>
-      <c r="E53" t="s">
-        <v>91</v>
+      <c r="E53" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -13549,8 +13554,8 @@
       <c r="D54" t="s">
         <v>132</v>
       </c>
-      <c r="E54" t="s">
-        <v>91</v>
+      <c r="E54" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -13566,7 +13571,7 @@
       <c r="D55" t="s">
         <v>133</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13583,7 +13588,7 @@
       <c r="D56" t="s">
         <v>134</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13600,7 +13605,7 @@
       <c r="D57" t="s">
         <v>135</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13617,7 +13622,7 @@
       <c r="D58" t="s">
         <v>136</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13634,7 +13639,7 @@
       <c r="D59" t="s">
         <v>137</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13651,7 +13656,7 @@
       <c r="D60" t="s">
         <v>138</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13668,7 +13673,7 @@
       <c r="D61" t="s">
         <v>139</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13685,7 +13690,7 @@
       <c r="D62" t="s">
         <v>140</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13702,8 +13707,8 @@
       <c r="D63" t="s">
         <v>141</v>
       </c>
-      <c r="E63" t="s">
-        <v>91</v>
+      <c r="E63" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -13719,7 +13724,7 @@
       <c r="D64" t="s">
         <v>142</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13736,7 +13741,7 @@
       <c r="D65" t="s">
         <v>143</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13753,7 +13758,7 @@
       <c r="D66" t="s">
         <v>144</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13770,7 +13775,7 @@
       <c r="D67" t="s">
         <v>145</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13787,7 +13792,7 @@
       <c r="D68" t="s">
         <v>146</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13804,7 +13809,7 @@
       <c r="D69" t="s">
         <v>147</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13821,8 +13826,8 @@
       <c r="D70" t="s">
         <v>148</v>
       </c>
-      <c r="E70" t="s">
-        <v>91</v>
+      <c r="E70" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -13838,8 +13843,8 @@
       <c r="D71" t="s">
         <v>149</v>
       </c>
-      <c r="E71" t="s">
-        <v>91</v>
+      <c r="E71" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -13855,8 +13860,8 @@
       <c r="D72" t="s">
         <v>150</v>
       </c>
-      <c r="E72" t="s">
-        <v>91</v>
+      <c r="E72" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -13872,7 +13877,7 @@
       <c r="D73" t="s">
         <v>151</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13889,7 +13894,7 @@
       <c r="D74" t="s">
         <v>152</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13906,7 +13911,7 @@
       <c r="D75" t="s">
         <v>153</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13923,7 +13928,7 @@
       <c r="D76" t="s">
         <v>154</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13940,7 +13945,7 @@
       <c r="D77" t="s">
         <v>155</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13957,7 +13962,7 @@
       <c r="D78" t="s">
         <v>156</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13974,7 +13979,7 @@
       <c r="D79" t="s">
         <v>157</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -13991,8 +13996,8 @@
       <c r="D80" t="s">
         <v>158</v>
       </c>
-      <c r="E80" t="s">
-        <v>91</v>
+      <c r="E80" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -14008,8 +14013,8 @@
       <c r="D81" t="s">
         <v>159</v>
       </c>
-      <c r="E81" t="s">
-        <v>92</v>
+      <c r="E81" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -14025,7 +14030,7 @@
       <c r="D82" t="s">
         <v>160</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14042,7 +14047,7 @@
       <c r="D83" t="s">
         <v>161</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14059,7 +14064,7 @@
       <c r="D84" t="s">
         <v>162</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14076,7 +14081,7 @@
       <c r="D85" t="s">
         <v>163</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14093,7 +14098,7 @@
       <c r="D86" t="s">
         <v>164</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14110,7 +14115,7 @@
       <c r="D87" t="s">
         <v>165</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14127,8 +14132,8 @@
       <c r="D88" t="s">
         <v>166</v>
       </c>
-      <c r="E88" t="s">
-        <v>92</v>
+      <c r="E88" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -14144,8 +14149,8 @@
       <c r="D89" t="s">
         <v>167</v>
       </c>
-      <c r="E89" t="s">
-        <v>92</v>
+      <c r="E89" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -14161,8 +14166,8 @@
       <c r="D90" t="s">
         <v>168</v>
       </c>
-      <c r="E90" t="s">
-        <v>92</v>
+      <c r="E90" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -14178,7 +14183,7 @@
       <c r="D91" t="s">
         <v>169</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14195,7 +14200,7 @@
       <c r="D92" t="s">
         <v>170</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14212,7 +14217,7 @@
       <c r="D93" t="s">
         <v>171</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14229,7 +14234,7 @@
       <c r="D94" t="s">
         <v>172</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14246,7 +14251,7 @@
       <c r="D95" t="s">
         <v>173</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14263,7 +14268,7 @@
       <c r="D96" t="s">
         <v>174</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14280,7 +14285,7 @@
       <c r="D97" t="s">
         <v>175</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14297,7 +14302,7 @@
       <c r="D98" t="s">
         <v>176</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14314,8 +14319,8 @@
       <c r="D99" t="s">
         <v>177</v>
       </c>
-      <c r="E99" t="s">
-        <v>92</v>
+      <c r="E99" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -14331,7 +14336,7 @@
       <c r="D100" t="s">
         <v>178</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14348,7 +14353,7 @@
       <c r="D101" t="s">
         <v>179</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14365,7 +14370,7 @@
       <c r="D102" t="s">
         <v>180</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14382,7 +14387,7 @@
       <c r="D103" t="s">
         <v>181</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E103" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14399,7 +14404,7 @@
       <c r="D104" t="s">
         <v>182</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14416,7 +14421,7 @@
       <c r="D105" t="s">
         <v>183</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E105" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -14433,8 +14438,8 @@
       <c r="D106" t="s">
         <v>184</v>
       </c>
-      <c r="E106" t="s">
-        <v>92</v>
+      <c r="E106" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -14450,8 +14455,8 @@
       <c r="D107" t="s">
         <v>185</v>
       </c>
-      <c r="E107" t="s">
-        <v>92</v>
+      <c r="E107" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -14467,8 +14472,8 @@
       <c r="D108" t="s">
         <v>268</v>
       </c>
-      <c r="E108" t="s">
-        <v>92</v>
+      <c r="E108" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -14484,7 +14489,7 @@
       <c r="D109" t="s">
         <v>270</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E109" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14501,8 +14506,8 @@
       <c r="D110" t="s">
         <v>271</v>
       </c>
-      <c r="E110" t="s">
-        <v>91</v>
+      <c r="E110" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -14518,8 +14523,8 @@
       <c r="D111" t="s">
         <v>272</v>
       </c>
-      <c r="E111" t="s">
-        <v>91</v>
+      <c r="E111" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -14535,8 +14540,8 @@
       <c r="D112" t="s">
         <v>273</v>
       </c>
-      <c r="E112" t="s">
-        <v>96</v>
+      <c r="E112" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -14552,7 +14557,7 @@
       <c r="D113" t="s">
         <v>274</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14569,7 +14574,7 @@
       <c r="D114" t="s">
         <v>275</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14586,7 +14591,7 @@
       <c r="D115" t="s">
         <v>276</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E115" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14603,7 +14608,7 @@
       <c r="D116" t="s">
         <v>277</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14620,8 +14625,8 @@
       <c r="D117" t="s">
         <v>278</v>
       </c>
-      <c r="E117" t="s">
-        <v>91</v>
+      <c r="E117" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -14637,8 +14642,8 @@
       <c r="D118" t="s">
         <v>279</v>
       </c>
-      <c r="E118" t="s">
-        <v>91</v>
+      <c r="E118" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -14654,8 +14659,8 @@
       <c r="D119" t="s">
         <v>280</v>
       </c>
-      <c r="E119" t="s">
-        <v>91</v>
+      <c r="E119" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -14671,7 +14676,7 @@
       <c r="D120" t="s">
         <v>281</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E120" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14688,7 +14693,7 @@
       <c r="D121" t="s">
         <v>282</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E121" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14705,7 +14710,7 @@
       <c r="D122" t="s">
         <v>283</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E122" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14722,7 +14727,7 @@
       <c r="D123" t="s">
         <v>284</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E123" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14739,7 +14744,7 @@
       <c r="D124" t="s">
         <v>285</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E124" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14756,7 +14761,7 @@
       <c r="D125" t="s">
         <v>286</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E125" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14773,7 +14778,7 @@
       <c r="D126" t="s">
         <v>287</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E126" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14790,7 +14795,7 @@
       <c r="D127" t="s">
         <v>288</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E127" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14807,8 +14812,8 @@
       <c r="D128" t="s">
         <v>289</v>
       </c>
-      <c r="E128" t="s">
-        <v>91</v>
+      <c r="E128" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -14824,7 +14829,7 @@
       <c r="D129" t="s">
         <v>290</v>
       </c>
-      <c r="E129" t="s">
+      <c r="E129" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14841,7 +14846,7 @@
       <c r="D130" t="s">
         <v>291</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E130" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14858,7 +14863,7 @@
       <c r="D131" t="s">
         <v>292</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E131" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14875,7 +14880,7 @@
       <c r="D132" t="s">
         <v>293</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E132" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14892,7 +14897,7 @@
       <c r="D133" t="s">
         <v>294</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E133" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14909,7 +14914,7 @@
       <c r="D134" t="s">
         <v>295</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E134" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14926,8 +14931,8 @@
       <c r="D135" t="s">
         <v>296</v>
       </c>
-      <c r="E135" t="s">
-        <v>91</v>
+      <c r="E135" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -14943,8 +14948,8 @@
       <c r="D136" t="s">
         <v>297</v>
       </c>
-      <c r="E136" t="s">
-        <v>91</v>
+      <c r="E136" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -14960,8 +14965,8 @@
       <c r="D137" t="s">
         <v>298</v>
       </c>
-      <c r="E137" t="s">
-        <v>91</v>
+      <c r="E137" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -14977,7 +14982,7 @@
       <c r="D138" t="s">
         <v>299</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E138" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -14994,7 +14999,7 @@
       <c r="D139" t="s">
         <v>300</v>
       </c>
-      <c r="E139" t="s">
+      <c r="E139" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15011,7 +15016,7 @@
       <c r="D140" t="s">
         <v>301</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15028,7 +15033,7 @@
       <c r="D141" t="s">
         <v>302</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E141" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15045,7 +15050,7 @@
       <c r="D142" t="s">
         <v>303</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E142" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15062,7 +15067,7 @@
       <c r="D143" t="s">
         <v>304</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E143" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15079,7 +15084,7 @@
       <c r="D144" t="s">
         <v>305</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E144" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15096,7 +15101,7 @@
       <c r="D145" t="s">
         <v>306</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E145" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15113,8 +15118,8 @@
       <c r="D146" t="s">
         <v>307</v>
       </c>
-      <c r="E146" t="s">
-        <v>91</v>
+      <c r="E146" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -15130,7 +15135,7 @@
       <c r="D147" t="s">
         <v>308</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E147" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15147,7 +15152,7 @@
       <c r="D148" t="s">
         <v>309</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E148" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15164,7 +15169,7 @@
       <c r="D149" t="s">
         <v>310</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E149" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15181,7 +15186,7 @@
       <c r="D150" t="s">
         <v>311</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E150" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15198,7 +15203,7 @@
       <c r="D151" t="s">
         <v>312</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E151" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15215,7 +15220,7 @@
       <c r="D152" t="s">
         <v>313</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E152" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15232,8 +15237,8 @@
       <c r="D153" t="s">
         <v>314</v>
       </c>
-      <c r="E153" t="s">
-        <v>91</v>
+      <c r="E153" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -15249,8 +15254,8 @@
       <c r="D154" t="s">
         <v>315</v>
       </c>
-      <c r="E154" t="s">
-        <v>91</v>
+      <c r="E154" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -15266,8 +15271,8 @@
       <c r="D155" t="s">
         <v>316</v>
       </c>
-      <c r="E155" t="s">
-        <v>91</v>
+      <c r="E155" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -15283,7 +15288,7 @@
       <c r="D156" t="s">
         <v>317</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E156" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15300,7 +15305,7 @@
       <c r="D157" t="s">
         <v>318</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E157" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15317,7 +15322,7 @@
       <c r="D158" t="s">
         <v>319</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E158" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15334,7 +15339,7 @@
       <c r="D159" t="s">
         <v>320</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E159" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15351,7 +15356,7 @@
       <c r="D160" t="s">
         <v>321</v>
       </c>
-      <c r="E160" t="s">
+      <c r="E160" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15368,7 +15373,7 @@
       <c r="D161" t="s">
         <v>322</v>
       </c>
-      <c r="E161" t="s">
+      <c r="E161" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15385,7 +15390,7 @@
       <c r="D162" t="s">
         <v>323</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E162" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15402,8 +15407,8 @@
       <c r="D163" t="s">
         <v>324</v>
       </c>
-      <c r="E163" t="s">
-        <v>91</v>
+      <c r="E163" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -15419,8 +15424,8 @@
       <c r="D164" t="s">
         <v>325</v>
       </c>
-      <c r="E164" t="s">
-        <v>92</v>
+      <c r="E164" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -15436,7 +15441,7 @@
       <c r="D165" t="s">
         <v>326</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15453,7 +15458,7 @@
       <c r="D166" t="s">
         <v>327</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15470,7 +15475,7 @@
       <c r="D167" t="s">
         <v>328</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15487,7 +15492,7 @@
       <c r="D168" t="s">
         <v>329</v>
       </c>
-      <c r="E168" t="s">
+      <c r="E168" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15504,7 +15509,7 @@
       <c r="D169" t="s">
         <v>330</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15521,7 +15526,7 @@
       <c r="D170" t="s">
         <v>331</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15538,8 +15543,8 @@
       <c r="D171" t="s">
         <v>332</v>
       </c>
-      <c r="E171" t="s">
-        <v>92</v>
+      <c r="E171" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -15555,8 +15560,8 @@
       <c r="D172" t="s">
         <v>333</v>
       </c>
-      <c r="E172" t="s">
-        <v>92</v>
+      <c r="E172" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -15572,8 +15577,8 @@
       <c r="D173" t="s">
         <v>334</v>
       </c>
-      <c r="E173" t="s">
-        <v>92</v>
+      <c r="E173" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -15589,7 +15594,7 @@
       <c r="D174" t="s">
         <v>335</v>
       </c>
-      <c r="E174" t="s">
+      <c r="E174" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15606,7 +15611,7 @@
       <c r="D175" t="s">
         <v>336</v>
       </c>
-      <c r="E175" t="s">
+      <c r="E175" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15623,7 +15628,7 @@
       <c r="D176" t="s">
         <v>337</v>
       </c>
-      <c r="E176" t="s">
+      <c r="E176" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15640,7 +15645,7 @@
       <c r="D177" t="s">
         <v>338</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15657,7 +15662,7 @@
       <c r="D178" t="s">
         <v>339</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15674,7 +15679,7 @@
       <c r="D179" t="s">
         <v>340</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15691,7 +15696,7 @@
       <c r="D180" t="s">
         <v>341</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15708,7 +15713,7 @@
       <c r="D181" t="s">
         <v>342</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15725,8 +15730,8 @@
       <c r="D182" t="s">
         <v>343</v>
       </c>
-      <c r="E182" t="s">
-        <v>92</v>
+      <c r="E182" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
@@ -15742,7 +15747,7 @@
       <c r="D183" t="s">
         <v>344</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15759,7 +15764,7 @@
       <c r="D184" t="s">
         <v>345</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15776,7 +15781,7 @@
       <c r="D185" t="s">
         <v>346</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15793,7 +15798,7 @@
       <c r="D186" t="s">
         <v>347</v>
       </c>
-      <c r="E186" t="s">
+      <c r="E186" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15810,7 +15815,7 @@
       <c r="D187" t="s">
         <v>348</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15827,7 +15832,7 @@
       <c r="D188" t="s">
         <v>349</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="4" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15844,8 +15849,8 @@
       <c r="D189" t="s">
         <v>350</v>
       </c>
-      <c r="E189" t="s">
-        <v>92</v>
+      <c r="E189" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
@@ -15861,8 +15866,8 @@
       <c r="D190" t="s">
         <v>351</v>
       </c>
-      <c r="E190" t="s">
-        <v>92</v>
+      <c r="E190" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
@@ -15878,8 +15883,8 @@
       <c r="D191" t="s">
         <v>352</v>
       </c>
-      <c r="E191" t="s">
-        <v>92</v>
+      <c r="E191" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -15895,7 +15900,7 @@
       <c r="D192" t="s">
         <v>542</v>
       </c>
-      <c r="E192" t="s">
+      <c r="E192" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15912,8 +15917,8 @@
       <c r="D193" t="s">
         <v>543</v>
       </c>
-      <c r="E193" t="s">
-        <v>91</v>
+      <c r="E193" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -15929,7 +15934,7 @@
       <c r="D194" t="s">
         <v>544</v>
       </c>
-      <c r="E194" t="s">
+      <c r="E194" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15946,8 +15951,8 @@
       <c r="D195" t="s">
         <v>545</v>
       </c>
-      <c r="E195" t="s">
-        <v>96</v>
+      <c r="E195" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
@@ -15963,7 +15968,7 @@
       <c r="D196" t="s">
         <v>546</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15980,7 +15985,7 @@
       <c r="D197" t="s">
         <v>547</v>
       </c>
-      <c r="E197" t="s">
+      <c r="E197" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15997,7 +16002,7 @@
       <c r="D198" t="s">
         <v>548</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E198" s="4" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
House can now be heated with heatingtype "HEATPUMP_GASPEAK"
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig_300.xlsx
+++ b/Base/db_backboneConfig_300.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405E2B53-BC96-4889-B05C-C7996D739D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A740359-C236-427B-897A-88F3EA96CA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18375" yWindow="3720" windowWidth="28470" windowHeight="16920" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="3615" yWindow="3090" windowWidth="28470" windowHeight="16920" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3810" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3810" uniqueCount="689">
   <si>
     <t>id</t>
   </si>
@@ -2104,6 +2104,9 @@
   </si>
   <si>
     <t>HEATPUMP_BOILERPEAK</t>
+  </si>
+  <si>
+    <t>HEATPUMP_GASPEAK</t>
   </si>
 </sst>
 </file>
@@ -2705,7 +2708,7 @@
   <dimension ref="A1:K303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2774,7 +2777,7 @@
         <v>657</v>
       </c>
       <c r="G2" t="s">
-        <v>651</v>
+        <v>688</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>

</xml_diff>